<commit_message>
adding to the literature review
</commit_message>
<xml_diff>
--- a/weeklyMeetings.xlsx
+++ b/weeklyMeetings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/46c66270056a4b13/Documents/UWE_CS_Y2/SD/GroupProject/systems-development-group-work/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="8_{C0FD7FFD-F558-49EB-8C7F-06976733FC5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E81AB6B2-73C8-409D-835A-9E15AA3ADE6F}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="8_{C0FD7FFD-F558-49EB-8C7F-06976733FC5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0A5FC836-F2E8-41C5-AF43-44AC8CC37A61}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="1" xr2:uid="{B8DBA4F2-B703-4988-8018-DA6ED3A2EFFF}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>Week</t>
   </si>
@@ -145,19 +145,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -177,6 +176,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -506,10 +509,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76D1F620-E331-4C9E-934B-517FB2723D8F}">
-  <dimension ref="A1:M20"/>
+  <dimension ref="B2:M20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="129" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -518,245 +521,242 @@
     <col min="3" max="3" width="16.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2" s="2"/>
-      <c r="B2" s="5" t="s">
+    <row r="2" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="E2" s="7" t="s">
+      <c r="C2" s="2"/>
+      <c r="E2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B3" s="6" t="s">
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+    </row>
+    <row r="3" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B4" s="6" t="s">
+      <c r="C3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B4" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="1"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B5" s="6" t="s">
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B5" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="1"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B6" s="6" t="s">
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B6" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="1"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B7" s="6" t="s">
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B7" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="1"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
-      <c r="L11" s="4"/>
-      <c r="M11" s="4"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
-      <c r="L12" s="4"/>
-      <c r="M12" s="4"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
-      <c r="L13" s="4"/>
-      <c r="M13" s="4"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
-      <c r="K14" s="4"/>
-      <c r="L14" s="4"/>
-      <c r="M14" s="4"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4"/>
-      <c r="K15" s="4"/>
-      <c r="L15" s="4"/>
-      <c r="M15" s="4"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="4"/>
-      <c r="K16" s="4"/>
-      <c r="L16" s="4"/>
-      <c r="M16" s="4"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5"/>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="5"/>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="5"/>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5"/>
+      <c r="M16" s="5"/>
     </row>
     <row r="17" spans="5:13" x14ac:dyDescent="0.3">
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
-      <c r="K17" s="4"/>
-      <c r="L17" s="4"/>
-      <c r="M17" s="4"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
+      <c r="M17" s="5"/>
     </row>
     <row r="18" spans="5:13" x14ac:dyDescent="0.3">
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
-      <c r="J18" s="4"/>
-      <c r="K18" s="4"/>
-      <c r="L18" s="4"/>
-      <c r="M18" s="4"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="5"/>
+      <c r="M18" s="5"/>
     </row>
     <row r="19" spans="5:13" x14ac:dyDescent="0.3">
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
-      <c r="K19" s="4"/>
-      <c r="L19" s="4"/>
-      <c r="M19" s="4"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="5"/>
+      <c r="M19" s="5"/>
     </row>
     <row r="20" spans="5:13" x14ac:dyDescent="0.3">
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="4"/>
-      <c r="K20" s="4"/>
-      <c r="L20" s="4"/>
-      <c r="M20" s="4"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="5"/>
+      <c r="L20" s="5"/>
+      <c r="M20" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
adding first meeting report
</commit_message>
<xml_diff>
--- a/weeklyMeetings.xlsx
+++ b/weeklyMeetings.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/46c66270056a4b13/Documents/UWE_CS_Y2/SD/GroupProject/systems-development-group-work/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="8_{C0FD7FFD-F558-49EB-8C7F-06976733FC5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0A5FC836-F2E8-41C5-AF43-44AC8CC37A61}"/>
+  <xr:revisionPtr revIDLastSave="81" documentId="8_{C0FD7FFD-F558-49EB-8C7F-06976733FC5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{49916153-81B3-488A-BECE-25D347B33463}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="1" xr2:uid="{B8DBA4F2-B703-4988-8018-DA6ED3A2EFFF}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="2" xr2:uid="{B8DBA4F2-B703-4988-8018-DA6ED3A2EFFF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" state="hidden" r:id="rId1"/>
     <sheet name="meetingTemplate" sheetId="1" r:id="rId2"/>
+    <sheet name="meeting1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,10 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
-  <si>
-    <t>Week</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="19">
   <si>
     <t>Team Coordinator</t>
   </si>
@@ -67,6 +65,36 @@
   </si>
   <si>
     <t>Meeting Report</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>The group has been completing the initial stages of the project.</t>
+  </si>
+  <si>
+    <t>Yasen has written the project planning, and has also begun looking at some code which we</t>
+  </si>
+  <si>
+    <t>could use for some of the system's funcitonality.</t>
+  </si>
+  <si>
+    <t>Will has written the project aims and objectives and contributed to the literature review.</t>
+  </si>
+  <si>
+    <t>He has also completed some early stages of the implementation, including a prototype GUI,</t>
+  </si>
+  <si>
+    <t>and has implemented the patient class.</t>
+  </si>
+  <si>
+    <t>Yamin and Shek worked together to identify the functional and non-funcitonal</t>
+  </si>
+  <si>
+    <t>requirements of the system.</t>
+  </si>
+  <si>
+    <t>I have been contributing to the literature review, and have made the Gantt chart.</t>
   </si>
 </sst>
 </file>
@@ -96,7 +124,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -141,11 +169,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -160,6 +225,19 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -489,17 +567,17 @@
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -511,8 +589,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76D1F620-E331-4C9E-934B-517FB2723D8F}">
   <dimension ref="B2:M20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="129" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView zoomScale="129" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8:M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -523,11 +601,11 @@
   <sheetData>
     <row r="2" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B2" s="3" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="C2" s="2"/>
       <c r="E2" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
@@ -540,228 +618,243 @@
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
+      <c r="C3" s="1"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="10"/>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B4" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4" s="1"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="10"/>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B5" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5" s="1"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="5"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="10"/>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B6" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6" s="1"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="5"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="10"/>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B7" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7" s="1"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="5"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="10"/>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="10"/>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
-      <c r="M9" s="5"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="10"/>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="5"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="10"/>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="5"/>
-      <c r="L11" s="5"/>
-      <c r="M11" s="5"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="10"/>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="5"/>
-      <c r="L12" s="5"/>
-      <c r="M12" s="5"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="10"/>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
-      <c r="K13" s="5"/>
-      <c r="L13" s="5"/>
-      <c r="M13" s="5"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="10"/>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="5"/>
-      <c r="L14" s="5"/>
-      <c r="M14" s="5"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="10"/>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
-      <c r="K15" s="5"/>
-      <c r="L15" s="5"/>
-      <c r="M15" s="5"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="9"/>
+      <c r="M15" s="10"/>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="5"/>
-      <c r="L16" s="5"/>
-      <c r="M16" s="5"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="10"/>
     </row>
     <row r="17" spans="5:13" x14ac:dyDescent="0.3">
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
-      <c r="M17" s="5"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="9"/>
+      <c r="M17" s="10"/>
     </row>
     <row r="18" spans="5:13" x14ac:dyDescent="0.3">
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="5"/>
-      <c r="L18" s="5"/>
-      <c r="M18" s="5"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
+      <c r="L18" s="9"/>
+      <c r="M18" s="10"/>
     </row>
     <row r="19" spans="5:13" x14ac:dyDescent="0.3">
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="5"/>
-      <c r="K19" s="5"/>
-      <c r="L19" s="5"/>
-      <c r="M19" s="5"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="9"/>
+      <c r="M19" s="10"/>
     </row>
     <row r="20" spans="5:13" x14ac:dyDescent="0.3">
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="5"/>
-      <c r="K20" s="5"/>
-      <c r="L20" s="5"/>
-      <c r="M20" s="5"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="9"/>
+      <c r="L20" s="9"/>
+      <c r="M20" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="E3:M20"/>
+  <mergeCells count="19">
+    <mergeCell ref="E17:M17"/>
+    <mergeCell ref="E18:M18"/>
+    <mergeCell ref="E19:M19"/>
+    <mergeCell ref="E20:M20"/>
     <mergeCell ref="E2:M2"/>
+    <mergeCell ref="E3:M3"/>
+    <mergeCell ref="E4:M4"/>
+    <mergeCell ref="E5:M5"/>
+    <mergeCell ref="E6:M6"/>
+    <mergeCell ref="E7:M7"/>
+    <mergeCell ref="E8:M8"/>
+    <mergeCell ref="E9:M9"/>
+    <mergeCell ref="E10:M10"/>
+    <mergeCell ref="E11:M11"/>
+    <mergeCell ref="E12:M12"/>
+    <mergeCell ref="E13:M13"/>
+    <mergeCell ref="E14:M14"/>
+    <mergeCell ref="E15:M15"/>
+    <mergeCell ref="E16:M16"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Enter a date." sqref="C2" xr:uid="{C24D4DCA-5549-449E-8ACB-08FD1420B262}">
@@ -784,4 +877,364 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6B1902D-478B-47F6-8A34-61E525337A8B}">
+  <dimension ref="B2:M23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="129" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17:M17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="7">
+        <v>45344</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+    </row>
+    <row r="3" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="E8" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="E9" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="E10" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="E12" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5"/>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="E13" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="10"/>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="E14" s="8"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="10"/>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="E15" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="9"/>
+      <c r="M15" s="10"/>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="E16" s="8"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="10"/>
+    </row>
+    <row r="17" spans="5:13" x14ac:dyDescent="0.3">
+      <c r="E17" s="8"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="9"/>
+      <c r="M17" s="10"/>
+    </row>
+    <row r="18" spans="5:13" x14ac:dyDescent="0.3">
+      <c r="E18" s="8"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
+      <c r="L18" s="9"/>
+      <c r="M18" s="10"/>
+    </row>
+    <row r="19" spans="5:13" x14ac:dyDescent="0.3">
+      <c r="E19" s="8"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="9"/>
+      <c r="M19" s="10"/>
+    </row>
+    <row r="20" spans="5:13" x14ac:dyDescent="0.3">
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="5"/>
+      <c r="L20" s="5"/>
+      <c r="M20" s="5"/>
+    </row>
+    <row r="21" spans="5:13" x14ac:dyDescent="0.3">
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="11"/>
+      <c r="J21" s="11"/>
+      <c r="K21" s="11"/>
+      <c r="L21" s="11"/>
+      <c r="M21" s="11"/>
+    </row>
+    <row r="22" spans="5:13" x14ac:dyDescent="0.3">
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="11"/>
+      <c r="J22" s="11"/>
+      <c r="K22" s="11"/>
+      <c r="L22" s="11"/>
+      <c r="M22" s="11"/>
+    </row>
+    <row r="23" spans="5:13" x14ac:dyDescent="0.3">
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="11"/>
+      <c r="J23" s="11"/>
+      <c r="K23" s="11"/>
+      <c r="L23" s="11"/>
+      <c r="M23" s="11"/>
+    </row>
+  </sheetData>
+  <mergeCells count="22">
+    <mergeCell ref="E4:M4"/>
+    <mergeCell ref="E20:M20"/>
+    <mergeCell ref="E21:M21"/>
+    <mergeCell ref="E22:M22"/>
+    <mergeCell ref="E23:M23"/>
+    <mergeCell ref="E11:M11"/>
+    <mergeCell ref="E7:M7"/>
+    <mergeCell ref="E14:M14"/>
+    <mergeCell ref="E15:M15"/>
+    <mergeCell ref="E16:M16"/>
+    <mergeCell ref="E17:M17"/>
+    <mergeCell ref="E18:M18"/>
+    <mergeCell ref="E19:M19"/>
+    <mergeCell ref="E2:M2"/>
+    <mergeCell ref="E3:M3"/>
+    <mergeCell ref="E5:M5"/>
+    <mergeCell ref="E6:M6"/>
+    <mergeCell ref="E8:M8"/>
+    <mergeCell ref="E9:M9"/>
+    <mergeCell ref="E10:M10"/>
+    <mergeCell ref="E12:M12"/>
+    <mergeCell ref="E13:M13"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Enter a date." sqref="C2" xr:uid="{B2300726-AD37-4201-9CE1-55C3F578E217}">
+      <formula1>45337</formula1>
+      <formula2>45427</formula2>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F79D1812-1379-4D27-8B84-5F1B0915B5A6}">
+          <x14:formula1>
+            <xm:f>Sheet2!$B$2:$B$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>C3:C7</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>